<commit_message>
Updated Catchment BC files
</commit_message>
<xml_diff>
--- a/matlab/WIR_Catchment/WIR Supporting Data.xlsx
+++ b/matlab/WIR_Catchment/WIR Supporting Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SCERM\matlab\WIR_Catchment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F575104B-F857-418D-9F53-8388CF8136F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218B986C-16DA-47A2-9885-93760D95A125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Site_Information" sheetId="1" r:id="rId1"/>
@@ -4147,7 +4147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4220,6 +4220,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4335,8 +4342,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4424,8 +4432,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{D88AE43C-F3F4-4EB3-8A74-133AC553AC80}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4705,7 +4714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A380" workbookViewId="0">
+    <sheetView topLeftCell="A380" workbookViewId="0">
       <selection activeCell="A414" sqref="A414"/>
     </sheetView>
   </sheetViews>
@@ -27710,13 +27719,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="B195" sqref="B195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -29811,6 +29821,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated WQ and Inflow files
</commit_message>
<xml_diff>
--- a/matlab/WIR_Catchment/WIR Supporting Data.xlsx
+++ b/matlab/WIR_Catchment/WIR Supporting Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SCERM\matlab\WIR_Catchment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218B986C-16DA-47A2-9885-93760D95A125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433323D3-743A-4FAB-9EDF-4384F435031A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-6225" windowWidth="16440" windowHeight="28590" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Site_Information" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2775" uniqueCount="1368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3003" uniqueCount="1439">
   <si>
     <t>SITE_ID</t>
   </si>
@@ -4141,6 +4141,219 @@
   </si>
   <si>
     <t>WQ_DIAG_TOT_TSS</t>
+  </si>
+  <si>
+    <t>Swan River - Guildford Rd Climate</t>
+  </si>
+  <si>
+    <t>s509619</t>
+  </si>
+  <si>
+    <t>Swan-Canning Estuary - Lwrswn - Waylen Buoy</t>
+  </si>
+  <si>
+    <t>s6167160</t>
+  </si>
+  <si>
+    <t>Cond @ 25 deg C (uS/cm)</t>
+  </si>
+  <si>
+    <t>Alkalinity (tot) (CaCO3) (ug/L)</t>
+  </si>
+  <si>
+    <t>Bottom Depth (m)</t>
+  </si>
+  <si>
+    <t>C (sol org) {DOC, DOC as NPOC} (ug/L)</t>
+  </si>
+  <si>
+    <t>Chlorophyll a (by vol) (mg/L)</t>
+  </si>
+  <si>
+    <t>Chlorophyll a (in situ) (ug/L)</t>
+  </si>
+  <si>
+    <t>Chlorophyll b (by vol) (mg/L)</t>
+  </si>
+  <si>
+    <t>Chlorophyll c (by vol) (mg/L)</t>
+  </si>
+  <si>
+    <t>Chlorophyll sample volume (mL)</t>
+  </si>
+  <si>
+    <t>Cloud cover (%)</t>
+  </si>
+  <si>
+    <t>Flow status (no units)</t>
+  </si>
+  <si>
+    <t>Fluorescence (V) (V)</t>
+  </si>
+  <si>
+    <t>N (org) (ug/L)</t>
+  </si>
+  <si>
+    <t>N (sum sol org) {DON} (ug/L)</t>
+  </si>
+  <si>
+    <t>N (sum sol ox) {NOx-N, TON} (ug/L)</t>
+  </si>
+  <si>
+    <t>N (tot kjel) {TKN} (ug/L)</t>
+  </si>
+  <si>
+    <t>N (tot) {TN, pTN} (ug/L)</t>
+  </si>
+  <si>
+    <t>NH3-N/NH4-N (sol) (ug/L)</t>
+  </si>
+  <si>
+    <t>O2-{DO %sat} (%)</t>
+  </si>
+  <si>
+    <t>O2-{DO conc} (mg/L)</t>
+  </si>
+  <si>
+    <t>P (tot) {TP, pTP} (ug/L)</t>
+  </si>
+  <si>
+    <t>pH (no units)</t>
+  </si>
+  <si>
+    <t>Phaeophytin a (by vol) (mg/L)</t>
+  </si>
+  <si>
+    <t>PO4-P (sol react) {SRP, FRP} (ug/L)</t>
+  </si>
+  <si>
+    <t>Salinity (ppt)</t>
+  </si>
+  <si>
+    <t>Secchi depth (m)</t>
+  </si>
+  <si>
+    <t>SiO2-Si (sol react) (ug/L)</t>
+  </si>
+  <si>
+    <t>Temperature (deg C)</t>
+  </si>
+  <si>
+    <t>Tide status (no units)</t>
+  </si>
+  <si>
+    <t>TSS (mg/L)</t>
+  </si>
+  <si>
+    <t>Turbidity (NTU) (NTU)</t>
+  </si>
+  <si>
+    <t>Wind direction (deg)</t>
+  </si>
+  <si>
+    <t>Wind speed (kn)</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>PSU</t>
+  </si>
+  <si>
+    <t>Alkalinity_Total_NEW</t>
+  </si>
+  <si>
+    <t>Bottom_Depth_NEW</t>
+  </si>
+  <si>
+    <t>C_Sol_NEW</t>
+  </si>
+  <si>
+    <t>Chlor_A_NEW</t>
+  </si>
+  <si>
+    <t>Chlor_A_insitu_NEW</t>
+  </si>
+  <si>
+    <t>Chlor_B_NEW</t>
+  </si>
+  <si>
+    <t>Chlor_C_NEW</t>
+  </si>
+  <si>
+    <t>Chlor_Vol_NEW</t>
+  </si>
+  <si>
+    <t>Cloud_Cover_NEW</t>
+  </si>
+  <si>
+    <t>Flow_Status_NEW</t>
+  </si>
+  <si>
+    <t>Fluorescence_NEW</t>
+  </si>
+  <si>
+    <t>ON_NEW</t>
+  </si>
+  <si>
+    <t>DON_NEW</t>
+  </si>
+  <si>
+    <t>NOx_mg_NEW</t>
+  </si>
+  <si>
+    <t>TKN_NEW</t>
+  </si>
+  <si>
+    <t>TN_NEW</t>
+  </si>
+  <si>
+    <t>NH3_NEW</t>
+  </si>
+  <si>
+    <t>DO_Percentage_NEW</t>
+  </si>
+  <si>
+    <t>DO_NEW</t>
+  </si>
+  <si>
+    <t>TP_NEW</t>
+  </si>
+  <si>
+    <t>pH_NEW</t>
+  </si>
+  <si>
+    <t>Parathion_NEW</t>
+  </si>
+  <si>
+    <t>PO4_NEW</t>
+  </si>
+  <si>
+    <t>Salinity_ppt_NEW</t>
+  </si>
+  <si>
+    <t>Secchi_NEW</t>
+  </si>
+  <si>
+    <t>SiO2_Si_NEW</t>
+  </si>
+  <si>
+    <t>Temperature_NEW</t>
+  </si>
+  <si>
+    <t>Tide_Status_NoUnits_NEW</t>
+  </si>
+  <si>
+    <t>TSS_NEW</t>
+  </si>
+  <si>
+    <t>Turbidity_NEW</t>
+  </si>
+  <si>
+    <t>Wind_Dir_NEW</t>
+  </si>
+  <si>
+    <t>Wind_Speed_NEW</t>
   </si>
 </sst>
 </file>
@@ -4346,7 +4559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4431,12 +4644,36 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{D88AE43C-F3F4-4EB3-8A74-133AC553AC80}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4714,8 +4951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1432"/>
   <sheetViews>
-    <sheetView topLeftCell="A380" workbookViewId="0">
-      <selection activeCell="A414" sqref="A414"/>
+    <sheetView topLeftCell="A374" workbookViewId="0">
+      <selection activeCell="A422" sqref="A422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -16981,13 +17218,57 @@
         <v>6457130</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A439" s="29"/>
-      <c r="B439" s="26"/>
-    </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A440" s="29"/>
-      <c r="B440" s="26"/>
+    <row r="439" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>509619</v>
+      </c>
+      <c r="B439">
+        <v>509619</v>
+      </c>
+      <c r="C439" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D439" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E439" s="11" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F439" s="11" t="s">
+        <v>1369</v>
+      </c>
+      <c r="G439">
+        <v>401828.07</v>
+      </c>
+      <c r="H439">
+        <v>6470114.1299999999</v>
+      </c>
+    </row>
+    <row r="440" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>6167160</v>
+      </c>
+      <c r="B440">
+        <v>6167160</v>
+      </c>
+      <c r="C440" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D440" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E440" s="11" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F440" s="11" t="s">
+        <v>1371</v>
+      </c>
+      <c r="G440">
+        <v>390828.64</v>
+      </c>
+      <c r="H440">
+        <v>6459103.9400000004</v>
+      </c>
     </row>
     <row r="441" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A441" s="29"/>
@@ -25518,15 +25799,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C231"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D196" sqref="D196"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="B200" sqref="B200:B231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="2"/>
   </cols>
@@ -27709,7 +27990,367 @@
         <v>38</v>
       </c>
     </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="32" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="32" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="32" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="32" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="32" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="32" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="32" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="32" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="32" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="32" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="32" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="32" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="32" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="32" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="32" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="32" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="32" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="32" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="32" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="32" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="32" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="32" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="32" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="32" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="32" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="32" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="32" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="32" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="32" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="32" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="32" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="32" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -27719,7 +28360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+    <sheetView topLeftCell="A165" workbookViewId="0">
       <selection activeCell="B195" sqref="B195"/>
     </sheetView>
   </sheetViews>
@@ -29827,10 +30468,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E205"/>
+  <dimension ref="A1:E238"/>
   <sheetViews>
-    <sheetView topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204:B204"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="B207" sqref="B207:B238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33052,7 +33693,557 @@
         <v>502</v>
       </c>
     </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B206" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C206" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D206" s="10">
+        <v>0</v>
+      </c>
+      <c r="E206" s="10" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="32" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C207" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D207" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="32" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C208" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D208" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="32" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C209" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="D209" s="10">
+        <f>1/12</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E209" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="32" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C210" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="D210" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E210" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="32" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C211" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D211" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E211" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="32" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C212" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D212" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E212" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="32" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C213" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D213" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E213" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="32" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C214" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D214" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E214" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="32" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C215" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="D215" s="10">
+        <v>1</v>
+      </c>
+      <c r="E215" s="10" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="32" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C216" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D216" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E216" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="32" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C217" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D217" s="10">
+        <v>1000</v>
+      </c>
+      <c r="E217" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="32" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D218" s="10">
+        <f>1/14</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="E218" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="32" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C219" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="D219" s="10">
+        <f>1/14</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="E219" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="32" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C220" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="D220" s="10">
+        <f>1/14</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="E220" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="32" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C221" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="D221" s="10">
+        <f>1/14</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="E221" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="32" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C222" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="D222" s="10">
+        <f>1/14</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="E222" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="32" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C223" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="D223" s="10">
+        <f>1/14</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="E223" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="32" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C224" s="8" t="s">
+        <v>562</v>
+      </c>
+      <c r="D224" s="8">
+        <v>1</v>
+      </c>
+      <c r="E224" s="8"/>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="32" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C225" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="D225" s="10">
+        <f>1000/32</f>
+        <v>31.25</v>
+      </c>
+      <c r="E225" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="32" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C226" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="D226" s="10">
+        <f>1/31</f>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="E226" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="32" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C227" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="D227" s="10">
+        <v>1</v>
+      </c>
+      <c r="E227" s="10"/>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="32" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C228" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D228" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="32" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C229" s="10" t="s">
+        <v>476</v>
+      </c>
+      <c r="D229" s="10">
+        <f>1/31</f>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="E229" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="32" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C230" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D230" s="8">
+        <v>1</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="32" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C231" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D231" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="32" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C232" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="D232" s="10">
+        <f>1/28.1</f>
+        <v>3.5587188612099641E-2</v>
+      </c>
+      <c r="E232" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="32" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C233" s="10" t="s">
+        <v>499</v>
+      </c>
+      <c r="D233" s="10">
+        <v>1</v>
+      </c>
+      <c r="E233" s="10" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="32" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C234" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D234" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="32" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C235" s="10" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D235" s="10">
+        <v>1</v>
+      </c>
+      <c r="E235" s="10" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="32" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C236" s="10" t="s">
+        <v>501</v>
+      </c>
+      <c r="D236" s="10">
+        <v>1</v>
+      </c>
+      <c r="E236" s="10" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="32" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C237" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D237" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="32" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C238" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D238" s="8">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A207:A238">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>